<commit_message>
Cleaned up and checked (update for layout files)
</commit_message>
<xml_diff>
--- a/_MUT_USERBIN/GWF.xlsx
+++ b/_MUT_USERBIN/GWF.xlsx
@@ -5,18 +5,31 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Grdbldr\MUT_Examples\_MUT_USERBIN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\source\repos\MUT_Examples\_MUT_USERBIN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCFF615-C707-4547-8DD8-D65B945BC74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4E89B6-8EA3-4FDF-B0F2-B52DE7DA753D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{122D133F-728C-41DF-B623-70CC6DE7E402}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{122D133F-728C-41DF-B623-70CC6DE7E402}"/>
   </bookViews>
   <sheets>
     <sheet name="GWF" sheetId="1" r:id="rId1"/>
     <sheet name="Options" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -766,9 +779,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -806,7 +819,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -912,7 +925,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1054,7 +1067,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1064,8 +1077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88C16DCD-FBFC-4CDF-A4BF-BCF0CDEB1753}">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1262,7 +1275,7 @@
         <v>18</v>
       </c>
       <c r="J4">
-        <v>3.34</v>
+        <v>3.3399999999999999E-2</v>
       </c>
       <c r="K4">
         <v>1.982</v>
@@ -1641,7 +1654,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="UM9O9WmK+vQYAWHgaKvL5AF2CXlGIcS3zLJXq3GkAIqA795fupyO7rG3oVXuQHvv1Pc9fNcOSFcuBkNlfEuh1w==" saltValue="2PanbMhfx2RmyYh+RhY9Sg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="DDANofhB180K5nR+ifSRUz4Qrv/GLzEBIwwR4WqhY+0PNXMQyFjLqVYaduMduypSlj/78JGRQ2JLfxKKL0fN0Q==" saltValue="+dITltPo7KRKZUDpRyh4dQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -1674,7 +1687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4CCE5A5-D02A-45E3-85E8-50E780745C47}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
superslab and v_catchment examples added
</commit_message>
<xml_diff>
--- a/_MUT_USERBIN/GWF.xlsx
+++ b/_MUT_USERBIN/GWF.xlsx
@@ -1,27 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Grdbldr\MUT_Examples\_MUT_USERBIN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SandBox\_MUT_USERBIN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C094850-13BA-4CBD-9B91-3CB9393ACBAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{960819B0-93FD-416D-B348-007A07512B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{122D133F-728C-41DF-B623-70CC6DE7E402}"/>
+    <workbookView xWindow="12600" yWindow="60" windowWidth="16200" windowHeight="7575" xr2:uid="{122D133F-728C-41DF-B623-70CC6DE7E402}"/>
   </bookViews>
   <sheets>
     <sheet name="GWF" sheetId="1" r:id="rId1"/>
     <sheet name="Options" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="50">
   <si>
     <t>Material ID</t>
   </si>
@@ -110,6 +123,9 @@
     <t>Rob copied these properties from the prototype VSF column  LPF file</t>
   </si>
   <si>
+    <t>Rob copied these properties from the prototype VSF Hillslope LPF file</t>
+  </si>
+  <si>
     <t>Length</t>
   </si>
   <si>
@@ -149,10 +165,25 @@
     <t>1D Column Brooks</t>
   </si>
   <si>
+    <t>2D Hillslope seconds</t>
+  </si>
+  <si>
     <t>3D Abduls Problem</t>
   </si>
   <si>
     <t>2D Hillslope 100 m length</t>
+  </si>
+  <si>
+    <t>Superslab soil</t>
+  </si>
+  <si>
+    <t>Copied from super_slab_case.mprops</t>
+  </si>
+  <si>
+    <t>Superslab slab1</t>
+  </si>
+  <si>
+    <t>Superslab slab2</t>
   </si>
 </sst>
 </file>
@@ -685,32 +716,24 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="42" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="42" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="42" applyFont="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1067,536 +1090,736 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88C16DCD-FBFC-4CDF-A4BF-BCF0CDEB1753}">
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="20" style="2" customWidth="1"/>
-    <col min="3" max="8" width="9.140625" style="2"/>
-    <col min="9" max="9" width="14.28515625" style="2" customWidth="1"/>
-    <col min="10" max="13" width="9.140625" style="2"/>
-    <col min="14" max="14" width="11.42578125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="46.7109375" style="2" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="10.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="20" style="4" customWidth="1"/>
+    <col min="3" max="8" width="9.140625" style="4"/>
+    <col min="9" max="9" width="14.28515625" style="4" customWidth="1"/>
+    <col min="10" max="13" width="9.140625" style="4"/>
+    <col min="14" max="14" width="11.42578125" style="4" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" style="4" customWidth="1"/>
+    <col min="16" max="16" width="46.7109375" style="4" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
+    <row r="2" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2">
+        <v>0.3</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="H2">
+        <v>0.43</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="K2">
+        <v>1.56</v>
+      </c>
+      <c r="L2">
+        <v>0.18140000000000001</v>
+      </c>
+      <c r="M2">
+        <v>6.5713999999999997</v>
+      </c>
+      <c r="N2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="8">
-        <v>0.3</v>
-      </c>
-      <c r="D2" s="8">
-        <v>10</v>
-      </c>
-      <c r="E2" s="8">
-        <v>10</v>
-      </c>
-      <c r="F2" s="8">
-        <v>0</v>
-      </c>
-      <c r="G2" s="8">
-        <v>9.9999999999999995E-8</v>
-      </c>
-      <c r="H2" s="8">
-        <v>0.43</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="8">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="K2" s="8">
-        <v>1.56</v>
-      </c>
-      <c r="L2" s="8">
-        <v>0.18140000000000001</v>
-      </c>
-      <c r="M2" s="8">
-        <v>6.5713999999999997</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="P2" s="9" t="s">
+      <c r="P2" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+    <row r="3" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3">
+        <v>0.3</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="H3">
+        <v>0.43</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="K3">
+        <v>1.56</v>
+      </c>
+      <c r="L3">
+        <v>0.18140000000000001</v>
+      </c>
+      <c r="M3">
+        <v>6.5713999999999997</v>
+      </c>
+      <c r="N3" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" t="s">
+        <v>39</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:A11" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="8">
-        <v>0.3</v>
-      </c>
-      <c r="D3" s="8">
-        <v>10</v>
-      </c>
-      <c r="E3" s="8">
-        <v>10</v>
-      </c>
-      <c r="F3" s="8">
-        <v>0</v>
-      </c>
-      <c r="G3" s="8">
+      <c r="C4">
+        <v>0.1</v>
+      </c>
+      <c r="D4">
+        <v>31.536000000000001</v>
+      </c>
+      <c r="E4">
+        <v>31.536000000000001</v>
+      </c>
+      <c r="F4">
+        <v>31.536000000000001</v>
+      </c>
+      <c r="G4">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="H3" s="8">
-        <v>0.43</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="8">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="K3" s="8">
-        <v>1.56</v>
-      </c>
-      <c r="L3" s="8">
-        <v>0.18140000000000001</v>
-      </c>
-      <c r="M3" s="8">
+      <c r="H4">
+        <v>0.1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4">
+        <v>3.3399999999999999E-2</v>
+      </c>
+      <c r="K4">
+        <v>1.982</v>
+      </c>
+      <c r="L4">
+        <v>0.27710000000000001</v>
+      </c>
+      <c r="M4">
         <v>6.5713999999999997</v>
       </c>
-      <c r="N3" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="P3" s="9" t="s">
+      <c r="N4" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
-        <f t="shared" ref="A4:A12" si="0">A3+1</f>
-        <v>3</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="D4" s="8">
-        <v>31.536000000000001</v>
-      </c>
-      <c r="E4" s="8">
-        <v>31.536000000000001</v>
-      </c>
-      <c r="F4" s="8">
-        <v>31.536000000000001</v>
-      </c>
-      <c r="G4" s="8">
-        <v>9.9999999999999995E-8</v>
-      </c>
-      <c r="H4" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="8">
-        <v>3.3399999999999999E-2</v>
-      </c>
-      <c r="K4" s="8">
-        <v>1.982</v>
-      </c>
-      <c r="L4" s="8">
-        <v>0.27710000000000001</v>
-      </c>
-      <c r="M4" s="8">
-        <v>6.5713999999999997</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="P4" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+    <row r="5" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="8">
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5">
         <v>0.3</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5">
         <v>1.47E-4</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5">
         <v>1.47E-4</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5">
         <v>0</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5">
         <v>1E-4</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5">
         <v>0.3</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5">
         <v>1</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5">
         <v>5</v>
       </c>
-      <c r="L5" s="8">
+      <c r="L5">
         <v>0.3</v>
       </c>
-      <c r="M5" s="8">
+      <c r="M5">
         <v>1</v>
       </c>
-      <c r="N5" s="8" t="s">
+      <c r="N5" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="8" t="s">
+      <c r="O5" t="s">
         <v>17</v>
       </c>
-      <c r="P5" s="9" t="s">
+      <c r="P5" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+    <row r="6" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="8">
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6">
         <v>0.34</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6">
         <v>0</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6">
         <v>1.1999999999999999E-7</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6">
         <v>0.34</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6">
         <v>1.9</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6">
         <v>6</v>
       </c>
-      <c r="L6" s="8">
+      <c r="L6">
         <v>0.18</v>
       </c>
-      <c r="M6" s="8">
+      <c r="M6">
         <v>1</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="N6" t="s">
         <v>16</v>
       </c>
-      <c r="O6" s="8" t="s">
+      <c r="O6" t="s">
         <v>17</v>
       </c>
-      <c r="P6" s="9" t="s">
+      <c r="P6" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+    <row r="7" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7">
         <v>0.34</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7">
         <v>0</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7">
         <v>1.1999999999999999E-7</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7">
         <v>0.34</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="8">
+      <c r="J7">
         <v>1.9</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7">
         <v>6</v>
       </c>
-      <c r="L7" s="8">
+      <c r="L7">
         <v>0.18</v>
       </c>
-      <c r="M7" s="8">
+      <c r="M7">
         <v>1</v>
       </c>
-      <c r="N7" s="8" t="s">
+      <c r="N7" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="8" t="s">
+      <c r="O7" t="s">
         <v>17</v>
       </c>
-      <c r="P7" s="9" t="s">
+      <c r="P7" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+    <row r="8" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8">
         <v>0.3</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8">
         <v>0</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8">
         <v>1E-4</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8">
         <v>0.3</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J8">
         <v>1</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K8">
         <v>5</v>
       </c>
-      <c r="L8" s="8">
+      <c r="L8">
         <v>0.3</v>
       </c>
-      <c r="M8" s="8">
+      <c r="M8">
         <v>1</v>
       </c>
-      <c r="N8" s="8" t="s">
+      <c r="N8" t="s">
         <v>16</v>
       </c>
-      <c r="O8" s="8" t="s">
+      <c r="O8" t="s">
         <v>17</v>
       </c>
-      <c r="P8" s="9" t="s">
+      <c r="P8" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+    <row r="9" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9">
         <v>0.5</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9">
         <v>1E-8</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9">
         <v>1E-8</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9">
         <v>0</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9">
         <v>1E-4</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9">
         <v>0.5</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J9">
         <v>1</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K9">
         <v>5</v>
       </c>
-      <c r="L9" s="8">
+      <c r="L9">
         <v>0.5</v>
       </c>
-      <c r="M9" s="8">
+      <c r="M9">
         <v>1</v>
       </c>
-      <c r="N9" s="8" t="s">
+      <c r="N9" t="s">
         <v>16</v>
       </c>
-      <c r="O9" s="8" t="s">
+      <c r="O9" t="s">
         <v>17</v>
       </c>
-      <c r="P9" s="9" t="s">
+      <c r="P9" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+    <row r="10" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10">
         <v>0.4</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10">
         <v>0</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10">
         <v>1E-4</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10">
         <v>0.4</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" t="s">
         <v>18</v>
       </c>
-      <c r="J10" s="8">
+      <c r="J10">
         <v>1</v>
       </c>
-      <c r="K10" s="8">
+      <c r="K10">
         <v>5</v>
       </c>
-      <c r="L10" s="8">
+      <c r="L10">
         <v>0.5</v>
       </c>
-      <c r="M10" s="8">
+      <c r="M10">
         <v>1</v>
       </c>
-      <c r="N10" s="8" t="s">
+      <c r="N10" t="s">
         <v>16</v>
       </c>
-      <c r="O10" s="8" t="s">
+      <c r="O10" t="s">
         <v>17</v>
       </c>
-      <c r="P10" s="9" t="s">
+      <c r="P10" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="P11" s="4"/>
+    <row r="11" spans="1:16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11">
+        <v>0.1</v>
+      </c>
+      <c r="D11">
+        <v>31.536000000000001</v>
+      </c>
+      <c r="E11">
+        <v>31.536000000000001</v>
+      </c>
+      <c r="F11">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="G11">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="H11">
+        <v>0.1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11">
+        <v>3.3399999999999999E-2</v>
+      </c>
+      <c r="K11">
+        <v>1.982</v>
+      </c>
+      <c r="L11">
+        <v>0.27710000000000001</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11" t="s">
+        <v>16</v>
+      </c>
+      <c r="O11" t="s">
+        <v>17</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="D12" s="4">
+        <v>10</v>
+      </c>
+      <c r="E12" s="4">
+        <v>10</v>
+      </c>
+      <c r="F12" s="4">
+        <v>10</v>
+      </c>
+      <c r="G12" s="6">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="4">
+        <v>6</v>
+      </c>
+      <c r="K12" s="4">
+        <v>2</v>
+      </c>
+      <c r="L12" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="M12" s="4">
+        <v>1</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="D13" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E13" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F13" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G13" s="4">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="H13" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="4">
+        <v>1</v>
+      </c>
+      <c r="K13" s="4">
+        <v>3</v>
+      </c>
+      <c r="L13" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="M13" s="4">
+        <v>1</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="F14" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="G14" s="4">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="H14" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="4">
+        <v>1</v>
+      </c>
+      <c r="K14" s="4">
+        <v>3</v>
+      </c>
+      <c r="L14" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="M14" s="4">
+        <v>1</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="P14" s="4" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="tTmTpaV4zcZSM1UVJkR7sYhVA+MysjqVeZUHeNy9oj8AV/PA8WcIBIsPz1K11dud12U9GHwsa8yUHvTjHi87/Q==" saltValue="roum0i+qFJboHBRoYu5v3g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="DDANofhB180K5nR+ifSRUz4Qrv/GLzEBIwwR4WqhY+0PNXMQyFjLqVYaduMduypSlj/78JGRQ2JLfxKKL0fN0Q==" saltValue="+dITltPo7KRKZUDpRyh4dQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -1637,13 +1860,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>10</v>
@@ -1651,13 +1874,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
@@ -1668,10 +1891,10 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
         <v>23</v>
@@ -1679,15 +1902,15 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
smith_woolhiser example and observation point layouts
</commit_message>
<xml_diff>
--- a/_MUT_USERBIN/GWF.xlsx
+++ b/_MUT_USERBIN/GWF.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Grdbldr\MUT_Examples\_MUT_USERBIN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE88C2B4-255D-4758-B6CE-D069B15A4B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1053F4FF-B876-43E7-A151-F5BA7134095E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="16200" xr2:uid="{122D133F-728C-41DF-B623-70CC6DE7E402}"/>
   </bookViews>
@@ -1108,8 +1108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88C16DCD-FBFC-4CDF-A4BF-BCF0CDEB1753}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1969,13 +1969,13 @@
         <v>18</v>
       </c>
       <c r="J17" s="6">
+        <v>4.4299999999999999E-2</v>
+      </c>
+      <c r="K17" s="6">
+        <v>4.3564999999999996</v>
+      </c>
+      <c r="L17" s="6">
         <v>5.2479999999999999E-2</v>
-      </c>
-      <c r="K17" s="6">
-        <v>4.4299999999999999E-2</v>
-      </c>
-      <c r="L17" s="6">
-        <v>4.3564999999999996</v>
       </c>
       <c r="M17" s="6">
         <v>1</v>
@@ -2195,7 +2195,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="gntfjQe+XDifTx9eDOs2bRTrovzuUad6zl9Yun72u6HitVz0a3TkYefeyG0C7OA7lRqge3j8E/MABhhPenBODQ==" saltValue="YhhLjfCsHP3bAb+TmQw7JQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="0NKnhfGWk2ssRoE/NG519MrPkU0fmOng6z6O5gpsDBnN9pGVR5pP7zaJxSklaDwOml2bW8qdAAiHqNX+feKvrw==" saltValue="bFiHxtdJeHJZpIOuWSsw5A==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <extLst>

</xml_diff>